<commit_message>
Database connector tests were updated
</commit_message>
<xml_diff>
--- a/docs/Tests.xlsx
+++ b/docs/Tests.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="260" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Database connector'!$C$1:$C$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Database connector'!$C$1:$C$36</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <t>void initializeDatabase()</t>
   </si>
@@ -262,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -322,6 +322,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -364,7 +375,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -376,6 +387,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -393,7 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -765,11 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:W42"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -791,7 +804,7 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="2" customFormat="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -820,7 +833,7 @@
       <c r="W2"/>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
-      <c r="A3" s="12"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
@@ -847,7 +860,7 @@
       <c r="W3"/>
     </row>
     <row r="4" spans="1:23" s="2" customFormat="1">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
@@ -874,7 +887,7 @@
       <c r="W4"/>
     </row>
     <row r="5" spans="1:23" s="2" customFormat="1">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
@@ -900,8 +913,8 @@
       <c r="V5"/>
       <c r="W5"/>
     </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:23" s="1" customFormat="1">
+      <c r="A6" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -932,8 +945,15 @@
       <c r="W6"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
@@ -956,8 +976,13 @@
       <c r="W7"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
@@ -980,8 +1005,15 @@
       <c r="W8"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
@@ -1004,8 +1036,13 @@
       <c r="W9"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
@@ -1028,8 +1065,15 @@
       <c r="W10"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
@@ -1052,8 +1096,13 @@
       <c r="W11"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
@@ -1075,12 +1124,10 @@
       <c r="V12"/>
       <c r="W12"/>
     </row>
-    <row r="13" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A13" s="9" t="s">
-        <v>2</v>
-      </c>
+    <row r="13" spans="1:23" s="1" customFormat="1">
+      <c r="A13" s="10"/>
       <c r="B13" s="5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>37</v>
@@ -1106,10 +1153,12 @@
       <c r="V13"/>
       <c r="W13"/>
     </row>
-    <row r="14" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A14" s="9"/>
+    <row r="14" spans="1:23" s="1" customFormat="1">
+      <c r="A14" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="B14" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>37</v>
@@ -1135,12 +1184,10 @@
       <c r="V14"/>
       <c r="W14"/>
     </row>
-    <row r="15" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A15" s="9" t="s">
-        <v>3</v>
-      </c>
+    <row r="15" spans="1:23" s="1" customFormat="1">
+      <c r="A15" s="10"/>
       <c r="B15" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>37</v>
@@ -1166,10 +1213,10 @@
       <c r="V15"/>
       <c r="W15"/>
     </row>
-    <row r="16" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:23" s="1" customFormat="1">
+      <c r="A16" s="10"/>
       <c r="B16" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>37</v>
@@ -1195,12 +1242,10 @@
       <c r="V16"/>
       <c r="W16"/>
     </row>
-    <row r="17" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A17" s="9" t="s">
-        <v>5</v>
-      </c>
+    <row r="17" spans="1:23" s="1" customFormat="1">
+      <c r="A17" s="10"/>
       <c r="B17" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>37</v>
@@ -1226,10 +1271,12 @@
       <c r="V17"/>
       <c r="W17"/>
     </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A18" s="9"/>
+    <row r="18" spans="1:23" s="1" customFormat="1">
+      <c r="A18" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="B18" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>37</v>
@@ -1255,10 +1302,10 @@
       <c r="V18"/>
       <c r="W18"/>
     </row>
-    <row r="19" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A19" s="9"/>
+    <row r="19" spans="1:23" s="1" customFormat="1">
+      <c r="A19" s="10"/>
       <c r="B19" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>37</v>
@@ -1284,12 +1331,10 @@
       <c r="V19"/>
       <c r="W19"/>
     </row>
-    <row r="20" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A20" s="9" t="s">
-        <v>6</v>
-      </c>
+    <row r="20" spans="1:23" s="1" customFormat="1">
+      <c r="A20" s="10"/>
       <c r="B20" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>37</v>
@@ -1315,10 +1360,10 @@
       <c r="V20"/>
       <c r="W20"/>
     </row>
-    <row r="21" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A21" s="9"/>
+    <row r="21" spans="1:23" s="1" customFormat="1">
+      <c r="A21" s="10"/>
       <c r="B21" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>37</v>
@@ -1344,10 +1389,10 @@
       <c r="V21"/>
       <c r="W21"/>
     </row>
-    <row r="22" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A22" s="9"/>
+    <row r="22" spans="1:23" s="1" customFormat="1">
+      <c r="A22" s="10"/>
       <c r="B22" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>37</v>
@@ -1373,10 +1418,12 @@
       <c r="V22"/>
       <c r="W22"/>
     </row>
-    <row r="23" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A23" s="9"/>
+    <row r="23" spans="1:23" s="1" customFormat="1">
+      <c r="A23" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="B23" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>37</v>
@@ -1402,12 +1449,10 @@
       <c r="V23"/>
       <c r="W23"/>
     </row>
-    <row r="24" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A24" s="9" t="s">
-        <v>7</v>
-      </c>
+    <row r="24" spans="1:23" s="1" customFormat="1">
+      <c r="A24" s="10"/>
       <c r="B24" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>37</v>
@@ -1433,10 +1478,10 @@
       <c r="V24"/>
       <c r="W24"/>
     </row>
-    <row r="25" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A25" s="9"/>
+    <row r="25" spans="1:23" s="1" customFormat="1">
+      <c r="A25" s="10"/>
       <c r="B25" s="5" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>37</v>
@@ -1462,10 +1507,10 @@
       <c r="V25"/>
       <c r="W25"/>
     </row>
-    <row r="26" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A26" s="9"/>
+    <row r="26" spans="1:23" s="1" customFormat="1">
+      <c r="A26" s="10"/>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>37</v>
@@ -1491,10 +1536,10 @@
       <c r="V26"/>
       <c r="W26"/>
     </row>
-    <row r="27" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A27" s="9"/>
+    <row r="27" spans="1:23" s="1" customFormat="1">
+      <c r="A27" s="10"/>
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>37</v>
@@ -1520,12 +1565,14 @@
       <c r="V27"/>
       <c r="W27"/>
     </row>
-    <row r="28" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A28" s="9"/>
-      <c r="B28" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="5" t="s">
+    <row r="28" spans="1:23" s="3" customFormat="1">
+      <c r="A28" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D28"/>
@@ -1549,14 +1596,14 @@
       <c r="V28"/>
       <c r="W28"/>
     </row>
-    <row r="29" spans="1:23" s="1" customFormat="1">
-      <c r="A29" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="5"/>
+    <row r="29" spans="1:23" s="3" customFormat="1">
+      <c r="A29" s="9"/>
+      <c r="B29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
@@ -1578,12 +1625,14 @@
       <c r="V29"/>
       <c r="W29"/>
     </row>
-    <row r="30" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A30" s="9"/>
-      <c r="B30" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="5" t="s">
+    <row r="30" spans="1:23" s="3" customFormat="1">
+      <c r="A30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D30"/>
@@ -1607,12 +1656,12 @@
       <c r="V30"/>
       <c r="W30"/>
     </row>
-    <row r="31" spans="1:23" s="1" customFormat="1" hidden="1">
-      <c r="A31" s="9"/>
-      <c r="B31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="5" t="s">
+    <row r="31" spans="1:23" s="3" customFormat="1">
+      <c r="A31" s="12"/>
+      <c r="B31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D31"/>
@@ -1636,12 +1685,16 @@
       <c r="V31"/>
       <c r="W31"/>
     </row>
-    <row r="32" spans="1:23" s="1" customFormat="1">
-      <c r="A32" s="9"/>
-      <c r="B32" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="5"/>
+    <row r="32" spans="1:23" s="3" customFormat="1">
+      <c r="A32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
@@ -1663,12 +1716,14 @@
       <c r="V32"/>
       <c r="W32"/>
     </row>
-    <row r="33" spans="1:23" s="1" customFormat="1">
+    <row r="33" spans="1:23" s="3" customFormat="1">
       <c r="A33" s="9"/>
-      <c r="B33" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="5"/>
+      <c r="B33" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="D33"/>
       <c r="E33"/>
       <c r="F33"/>
@@ -1690,12 +1745,10 @@
       <c r="V33"/>
       <c r="W33"/>
     </row>
-    <row r="34" spans="1:23" s="3" customFormat="1" hidden="1">
-      <c r="A34" s="14" t="s">
-        <v>9</v>
-      </c>
+    <row r="34" spans="1:23" s="3" customFormat="1">
+      <c r="A34" s="9"/>
       <c r="B34" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>37</v>
@@ -1721,10 +1774,12 @@
       <c r="V34"/>
       <c r="W34"/>
     </row>
-    <row r="35" spans="1:23" s="3" customFormat="1" hidden="1">
-      <c r="A35" s="14"/>
+    <row r="35" spans="1:23" s="3" customFormat="1">
+      <c r="A35" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="B35" s="6" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>37</v>
@@ -1750,12 +1805,10 @@
       <c r="V35"/>
       <c r="W35"/>
     </row>
-    <row r="36" spans="1:23" s="3" customFormat="1" hidden="1">
-      <c r="A36" s="10" t="s">
-        <v>10</v>
-      </c>
+    <row r="36" spans="1:23" s="3" customFormat="1">
+      <c r="A36" s="9"/>
       <c r="B36" s="6" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>37</v>
@@ -1781,202 +1834,20 @@
       <c r="V36"/>
       <c r="W36"/>
     </row>
-    <row r="37" spans="1:23" s="3" customFormat="1" hidden="1">
-      <c r="A37" s="11"/>
-      <c r="B37" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37"/>
-      <c r="M37"/>
-      <c r="N37"/>
-      <c r="O37"/>
-      <c r="P37"/>
-      <c r="Q37"/>
-      <c r="R37"/>
-      <c r="S37"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-    </row>
-    <row r="38" spans="1:23" s="3" customFormat="1" hidden="1">
-      <c r="A38" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38"/>
-      <c r="N38"/>
-      <c r="O38"/>
-      <c r="P38"/>
-      <c r="Q38"/>
-      <c r="R38"/>
-      <c r="S38"/>
-      <c r="T38"/>
-      <c r="U38"/>
-      <c r="V38"/>
-      <c r="W38"/>
-    </row>
-    <row r="39" spans="1:23" s="3" customFormat="1" hidden="1">
-      <c r="A39" s="14"/>
-      <c r="B39" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39"/>
-      <c r="N39"/>
-      <c r="O39"/>
-      <c r="P39"/>
-      <c r="Q39"/>
-      <c r="R39"/>
-      <c r="S39"/>
-      <c r="T39"/>
-      <c r="U39"/>
-      <c r="V39"/>
-      <c r="W39"/>
-    </row>
-    <row r="40" spans="1:23" s="3" customFormat="1" hidden="1">
-      <c r="A40" s="14"/>
-      <c r="B40" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40"/>
-      <c r="N40"/>
-      <c r="O40"/>
-      <c r="P40"/>
-      <c r="Q40"/>
-      <c r="R40"/>
-      <c r="S40"/>
-      <c r="T40"/>
-      <c r="U40"/>
-      <c r="V40"/>
-      <c r="W40"/>
-    </row>
-    <row r="41" spans="1:23" s="3" customFormat="1" hidden="1">
-      <c r="A41" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
-      <c r="M41"/>
-      <c r="N41"/>
-      <c r="O41"/>
-      <c r="P41"/>
-      <c r="Q41"/>
-      <c r="R41"/>
-      <c r="S41"/>
-      <c r="T41"/>
-      <c r="U41"/>
-      <c r="V41"/>
-      <c r="W41"/>
-    </row>
-    <row r="42" spans="1:23" s="3" customFormat="1" hidden="1">
-      <c r="A42" s="14"/>
-      <c r="B42" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42"/>
-      <c r="E42"/>
-      <c r="F42"/>
-      <c r="G42"/>
-      <c r="H42"/>
-      <c r="I42"/>
-      <c r="J42"/>
-      <c r="K42"/>
-      <c r="L42"/>
-      <c r="M42"/>
-      <c r="N42"/>
-      <c r="O42"/>
-      <c r="P42"/>
-      <c r="Q42"/>
-      <c r="R42"/>
-      <c r="S42"/>
-      <c r="T42"/>
-      <c r="U42"/>
-      <c r="V42"/>
-      <c r="W42"/>
-    </row>
   </sheetData>
-  <autoFilter ref="C1:C42">
-    <filterColumn colId="0">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="C1:C36"/>
   <mergeCells count="11">
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A30:A31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>